<commit_message>
add materials for session 12
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/25-1-be/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52F7422-D550-EB42-86DF-880AB6666D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE51C25D-DDC8-204C-B630-C304B0328197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10900" yWindow="5460" windowWidth="29400" windowHeight="18360" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>exercises/e05.html</t>
+  </si>
+  <si>
+    <t>https://stats.ifp.uni-mainz.de/ba-ccs-track/befragung-rewb.html</t>
+  </si>
+  <si>
+    <t>exercises/e12.html</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -704,6 +710,12 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">

</xml_diff>

<commit_message>
add slides and links
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/25-1-be/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE51C25D-DDC8-204C-B630-C304B0328197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0609AF91-3AF5-3645-9CA5-D5FF3543DBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="5460" windowWidth="29400" windowHeight="18360" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>exercises/e12.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-14-semesterabschluss-und-informationen-zum-projektbericht</t>
+  </si>
+  <si>
+    <t>https://stats.ifp.uni-mainz.de/ba-ccs-track/befragung-linkage.html</t>
   </si>
 </sst>
 </file>
@@ -179,12 +185,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -502,7 +509,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,6 +706,9 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
+      <c r="F12" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -727,6 +737,9 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -737,6 +750,9 @@
       </c>
       <c r="C15" t="s">
         <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>

</xml_diff>